<commit_message>
add slicer and update design
</commit_message>
<xml_diff>
--- a/!webprog-asset.xlsx
+++ b/!webprog-asset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diva Angelika\DIVA\BINUS\Diva - Materi Kuliah\Semester 5\Web Programming\LAB\!WEBPROG LAB PROJECT\Assets in Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diva Angelika\DIVA\GitHub\webprog-lab-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621C0CBA-92E3-4D25-8FE0-2D74EE7544F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8204E703-72E0-4562-BBF7-4C390DE476E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,9 +18,18 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$E$1:$F$1</definedName>
+    <definedName name="Slicer_movie_title">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
+      <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicerCache r:id="rId3"/>
+      </x15:slicerCaches>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -1638,27 +1647,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1681,40 +1678,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1724,11 +1797,254 @@
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="fill" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1739,6 +2055,120 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19474</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>575733</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="movie-title">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB445540-AFB6-2BB0-5317-50D1746C485E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="movie-title"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13525499" y="214207"/>
+              <a:ext cx="5219701" cy="5052060"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_movie_title" xr10:uid="{5F517A80-5B74-405B-9E15-D87B971C77A7}" sourceName="movie-title">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="1"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="movie-title" xr10:uid="{08B2BEE7-2FF1-4025-9335-875D9CD6B98F}" cache="Slicer_movie_title" caption="movie-title" style="SlicerStyleLight2" rowHeight="260350"/>
+</slicers>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F0D0098-3E62-4BE0-B62F-FD03DA48BE22}" name="Table2" displayName="Table2" ref="A1:F101" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:F101" xr:uid="{3F0D0098-3E62-4BE0-B62F-FD03DA48BE22}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{19B0A467-D2C2-4CB7-8FA2-7BAA3617FAEC}" name="movie-title" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6064463C-B373-4DB4-A8B8-062B04C2177A}" name="web-link-href" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{604A368D-B33B-4024-A575-11321898CAE6}" name="movie-synopsis" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{369B4A82-AA83-4E9F-AF62-4D0D74373029}" name="movie-posters-link-src" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{FDC0DF83-AAEA-40DC-B7E9-91CBB224AF35}" name="cast1" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{4C7275B6-1EE4-494F-8EC9-846CCCABC0B1}" name="role1" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2040,9 +2470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2050,2038 +2480,2048 @@
     <col min="1" max="1" width="48.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.796875" customWidth="1"/>
     <col min="3" max="3" width="16.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="12" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="17" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="16" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="17" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="17" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="17" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="17" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="17" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="17" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="17" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="17" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="17" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="17" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="17" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="17" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="17" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="17" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="16" t="s">
         <v>411</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="16" t="s">
         <v>412</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="17" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="17" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="16" t="s">
         <v>416</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="17" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="16" t="s">
         <v>418</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="17" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="16" t="s">
         <v>420</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="17" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="17" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="17" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="17" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="17" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="16" t="s">
         <v>428</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="17" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="16" t="s">
         <v>430</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="17" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="17" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="17" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="16" t="s">
         <v>430</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="17" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="17" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="16" t="s">
         <v>436</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="17" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="17" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="16" t="s">
         <v>438</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="16" t="s">
         <v>436</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="17" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="17" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="17" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="17" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="16" t="s">
         <v>441</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="17" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="17" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="17" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="17" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="16" t="s">
         <v>447</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" s="17" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="16" t="s">
         <v>449</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="17" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="17" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="17" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F49" s="17" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="17" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="17" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="17" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="16" t="s">
         <v>456</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F53" s="17" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F54" s="17" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="16" t="s">
         <v>459</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" s="17" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F56" s="17" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="16" t="s">
         <v>461</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" s="17" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F58" s="17" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="16" t="s">
         <v>464</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F59" s="17" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="F60" s="17" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E61" s="16" t="s">
         <v>467</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="F61" s="17" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="F62" s="8" t="s">
+      <c r="F62" s="17" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F63" s="17" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E64" s="16" t="s">
         <v>471</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="F64" s="17" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E65" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F65" s="17" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E66" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="F66" s="17" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E67" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="F67" s="17" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E68" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F68" s="17" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E69" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="F69" s="8" t="s">
+      <c r="F69" s="17" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E70" s="16" t="s">
         <v>456</v>
       </c>
-      <c r="F70" s="8" t="s">
+      <c r="F70" s="17" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="16" t="s">
         <v>480</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="F71" s="17" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E72" s="16" t="s">
         <v>428</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F72" s="17" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F73" s="17" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E74" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="17" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E75" s="16" t="s">
         <v>484</v>
       </c>
-      <c r="F75" s="8" t="s">
+      <c r="F75" s="17" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E76" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="F76" s="8" t="s">
+      <c r="F76" s="17" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="E77" s="8" t="s">
+      <c r="E77" s="16" t="s">
         <v>487</v>
       </c>
-      <c r="F77" s="8" t="s">
+      <c r="F77" s="17" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="E78" s="8" t="s">
+      <c r="E78" s="16" t="s">
         <v>489</v>
       </c>
-      <c r="F78" s="8" t="s">
+      <c r="F78" s="17" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="E79" s="8" t="s">
+      <c r="E79" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="F79" s="8" t="s">
+      <c r="F79" s="17" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="E80" s="8" t="s">
+      <c r="E80" s="16" t="s">
         <v>492</v>
       </c>
-      <c r="F80" s="8" t="s">
+      <c r="F80" s="17" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="E81" s="8" t="s">
+      <c r="E81" s="16" t="s">
         <v>384</v>
       </c>
-      <c r="F81" s="8" t="s">
+      <c r="F81" s="17" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="E82" s="8" t="s">
+      <c r="E82" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="F82" s="17" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="E83" s="8" t="s">
+      <c r="E83" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="F83" s="8" t="s">
+      <c r="F83" s="17" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="E84" s="8" t="s">
+      <c r="E84" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="F84" s="17" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="E85" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="F85" s="8" t="s">
+      <c r="F85" s="17" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="E86" s="8" t="s">
+      <c r="E86" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="F86" s="8" t="s">
+      <c r="F86" s="17" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="F87" s="17" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E88" s="16" t="s">
         <v>501</v>
       </c>
-      <c r="F88" s="8" t="s">
+      <c r="F88" s="17" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="16" t="s">
         <v>503</v>
       </c>
-      <c r="F89" s="8" t="s">
+      <c r="F89" s="17" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D90" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="E90" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="F90" s="8" t="s">
+      <c r="F90" s="17" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D91" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E91" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="F91" s="8" t="s">
+      <c r="F91" s="17" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="E92" s="16" t="s">
         <v>384</v>
       </c>
-      <c r="F92" s="8" t="s">
+      <c r="F92" s="17" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="E93" s="8" t="s">
+      <c r="E93" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="F93" s="8" t="s">
+      <c r="F93" s="17" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="E94" s="8" t="s">
+      <c r="E94" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="F94" s="8" t="s">
+      <c r="F94" s="17" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="E95" s="8" t="s">
+      <c r="E95" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="F95" s="8" t="s">
+      <c r="F95" s="17" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="E96" s="8" t="s">
+      <c r="E96" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F96" s="17" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="E97" s="16" t="s">
         <v>492</v>
       </c>
-      <c r="F97" s="8" t="s">
+      <c r="F97" s="17" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="E98" s="8" t="s">
+      <c r="E98" s="16" t="s">
         <v>510</v>
       </c>
-      <c r="F98" s="8" t="s">
+      <c r="F98" s="17" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="E99" s="8" t="s">
+      <c r="E99" s="16" t="s">
         <v>512</v>
       </c>
-      <c r="F99" s="8" t="s">
+      <c r="F99" s="17" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="D100" s="5"/>
-      <c r="E100" s="8" t="s">
+      <c r="D100" s="19"/>
+      <c r="E100" s="16" t="s">
         <v>492</v>
       </c>
-      <c r="F100" s="8" t="s">
+      <c r="F100" s="17" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C101" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="D101" s="5"/>
-      <c r="E101" s="8" t="s">
+      <c r="D101" s="23"/>
+      <c r="E101" s="24" t="s">
         <v>514</v>
       </c>
-      <c r="F101" s="8" t="s">
+      <c r="F101" s="25" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C102" s="13"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="15" t="s">
+    <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="5"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="7" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
+      <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4089,7 +4529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998407B4-5459-4A42-A654-39EB44BCADB1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>